<commit_message>
Wrong part number identified and corrected IC1, IC2, IC3 and IC4
The AD8039 was incorrectly tagged as an AD8033 in the extended description fields and in the BOM spreadsheet. This has now been corrected. Based on production testing, analogue units with the AD8033 IC's fitted are still functional with the Cosmic Pi Main Board V2.5 production units. I'm not entirely sure why/how they still work, but it's been tested (stack/unstack - https://www.youtube.com/watch?v=crR5aZPUKPI), and they do.
</commit_message>
<xml_diff>
--- a/AnalogueProductionBOM.xlsx
+++ b/AnalogueProductionBOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cern.ch\dfs\Users\j\jdevine\Desktop\Cosmic Pi Analogue V2.4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cern.ch\dfs\Users\j\jdevine\Documents\Cosmic Pi Analogue V2.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -252,24 +252,12 @@
     <t>AD8039</t>
   </si>
   <si>
-    <t>AD8033R</t>
-  </si>
-  <si>
     <t>SO8</t>
   </si>
   <si>
     <t>IC1, IC2</t>
   </si>
   <si>
-    <t>2.7 V, 800 ?A, 80 MHz Rail-to-Rail I/O Amplifiers</t>
-  </si>
-  <si>
-    <t>ALTERA CORPORATION</t>
-  </si>
-  <si>
-    <t>AD8033ARZ</t>
-  </si>
-  <si>
     <t>BAS70-04</t>
   </si>
   <si>
@@ -403,17 +391,37 @@
   </si>
   <si>
     <t>LTST-S270TBKT-5A</t>
+  </si>
+  <si>
+    <t>Analogue Devices</t>
+  </si>
+  <si>
+    <t>AD8039ARZ</t>
+  </si>
+  <si>
+    <t>AD8039R</t>
+  </si>
+  <si>
+    <t>Low Power, 350 MHz Voltage Feedback Amplifiers, 3V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -441,13 +449,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,16 +774,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -786,10 +795,10 @@
         <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="M1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -806,7 +815,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
@@ -815,10 +824,10 @@
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -835,7 +844,7 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I3">
         <v>744235601</v>
@@ -847,10 +856,10 @@
         <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -870,7 +879,7 @@
         <v>0.1</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
@@ -879,10 +888,10 @@
         <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -902,7 +911,7 @@
         <v>0.2</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -911,10 +920,10 @@
         <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -934,7 +943,7 @@
         <v>0.1</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J6" t="s">
         <v>30</v>
@@ -943,10 +952,10 @@
         <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -966,7 +975,7 @@
         <v>1E-3</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -975,10 +984,10 @@
         <v>32</v>
       </c>
       <c r="L7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -998,7 +1007,7 @@
         <v>0.1</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J8" t="s">
         <v>21</v>
@@ -1007,10 +1016,10 @@
         <v>18</v>
       </c>
       <c r="L8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1030,7 +1039,7 @@
         <v>0.01</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -1039,10 +1048,10 @@
         <v>38</v>
       </c>
       <c r="L9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1062,7 +1071,7 @@
         <v>0.01</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J10" t="s">
         <v>11</v>
@@ -1071,10 +1080,10 @@
         <v>8</v>
       </c>
       <c r="L10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1094,7 +1103,7 @@
         <v>0.1</v>
       </c>
       <c r="G11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J11" t="s">
         <v>21</v>
@@ -1103,10 +1112,10 @@
         <v>18</v>
       </c>
       <c r="L11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1126,7 +1135,7 @@
         <v>0.1</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J12" t="s">
         <v>21</v>
@@ -1135,10 +1144,10 @@
         <v>45</v>
       </c>
       <c r="L12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1158,7 +1167,7 @@
         <v>0.1</v>
       </c>
       <c r="G13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J13" t="s">
         <v>21</v>
@@ -1167,10 +1176,10 @@
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1190,7 +1199,7 @@
         <v>0.01</v>
       </c>
       <c r="F14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J14" t="s">
         <v>11</v>
@@ -1199,10 +1208,10 @@
         <v>38</v>
       </c>
       <c r="L14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1231,10 +1240,10 @@
         <v>51</v>
       </c>
       <c r="L15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1263,10 +1272,10 @@
         <v>55</v>
       </c>
       <c r="L16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1286,7 +1295,7 @@
         <v>0.01</v>
       </c>
       <c r="F17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J17" t="s">
         <v>11</v>
@@ -1295,10 +1304,10 @@
         <v>38</v>
       </c>
       <c r="L17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1318,7 +1327,7 @@
         <v>0.05</v>
       </c>
       <c r="G18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J18" t="s">
         <v>21</v>
@@ -1327,10 +1336,10 @@
         <v>18</v>
       </c>
       <c r="L18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1341,7 +1350,7 @@
         <v>330</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -1350,7 +1359,7 @@
         <v>0.01</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J19" t="s">
         <v>11</v>
@@ -1359,10 +1368,10 @@
         <v>38</v>
       </c>
       <c r="L19" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1382,7 +1391,7 @@
         <v>0.01</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J20" t="s">
         <v>11</v>
@@ -1391,42 +1400,42 @@
         <v>38</v>
       </c>
       <c r="L20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H21" t="s">
-        <v>68</v>
-      </c>
-      <c r="I21" t="s">
-        <v>69</v>
-      </c>
-      <c r="J21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="D21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L21" t="s">
-        <v>93</v>
-      </c>
-      <c r="M21" t="s">
-        <v>94</v>
+      <c r="H21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1434,31 +1443,31 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -1466,31 +1475,31 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1498,31 +1507,31 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" t="s">
         <v>78</v>
       </c>
-      <c r="C24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" t="s">
-        <v>79</v>
-      </c>
-      <c r="H24" t="s">
-        <v>82</v>
-      </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L24" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1530,31 +1539,32 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>